<commit_message>
Created CPU entity, added CPU tests, tested commands
</commit_message>
<xml_diff>
--- a/doc/ALUmapping.xlsx
+++ b/doc/ALUmapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="44">
   <si>
     <t>Instruction</t>
   </si>
@@ -146,13 +146,7 @@
 </t>
   </si>
   <si>
-    <t>CMPi</t>
-  </si>
-  <si>
-    <t>PSR &lt;= (Param1 &lt; Param2)</t>
-  </si>
-  <si>
-    <t>.</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -298,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,8 +315,8 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,6 +331,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -662,23 +665,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="18" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="18" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1263,11 +1266,11 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>44</v>
+      <c r="B12" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="12"/>
@@ -1282,12 +1285,12 @@
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="12" t="s">
-        <v>45</v>
+      <c r="A13" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
@@ -1303,8 +1306,8 @@
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
       <c r="O13" s="7"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="12"/>
@@ -1322,8 +1325,8 @@
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="12"/>
@@ -1341,8 +1344,8 @@
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="7"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="12"/>
@@ -1360,8 +1363,8 @@
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
       <c r="O16" s="7"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="12"/>
@@ -1379,8 +1382,8 @@
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="7"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="12"/>
@@ -1398,8 +1401,8 @@
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
       <c r="O18" s="7"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="12"/>
@@ -1417,8 +1420,8 @@
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
       <c r="O19" s="7"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update CPU instructions-handling-unit with new entities and test cases
</commit_message>
<xml_diff>
--- a/doc/ALUmapping.xlsx
+++ b/doc/ALUmapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="44">
   <si>
     <t>Instruction</t>
   </si>
@@ -146,7 +146,7 @@
 </t>
   </si>
   <si>
-    <t/>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -154,7 +154,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,12 +165,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -292,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,7 +309,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
@@ -336,15 +330,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -355,7 +340,7 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,23 +650,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="18" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="15" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1261,17 +1246,13 @@
       <c r="P11" s="14">
         <v>1</v>
       </c>
-      <c r="Q11" s="14">
-        <v>1</v>
+      <c r="Q11" s="14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>43</v>
-      </c>
+      <c r="A12" s="12"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="12"/>
       <c r="E12" s="10"/>
@@ -1285,13 +1266,11 @@
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A13" s="12"/>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
@@ -1306,8 +1285,8 @@
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
       <c r="O13" s="7"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="12"/>
@@ -1325,8 +1304,8 @@
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="12"/>
@@ -1344,8 +1323,8 @@
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="7"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="12"/>
@@ -1363,8 +1342,8 @@
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
       <c r="O16" s="7"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="12"/>
@@ -1382,8 +1361,8 @@
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="7"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="12"/>
@@ -1401,8 +1380,8 @@
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
       <c r="O18" s="7"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="12"/>
@@ -1420,8 +1399,8 @@
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
       <c r="O19" s="7"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>